<commit_message>
modify 00 and 01, adding Vietnamese_text normalize
</commit_message>
<xml_diff>
--- a/Datasets/Raw_data/Unemployed_data.xlsx
+++ b/Datasets/Raw_data/Unemployed_data.xlsx
@@ -1,26 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29231"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Documents\Uni\FPT_Subjects\Fall_2025\ADY201m\Final\Datasets\Raw_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8ED40149-380C-4F5F-80BE-AC4E66E8D9AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E259C57-C665-4E94-8DAC-585D483979A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1966" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1966" uniqueCount="76">
   <si>
     <t>Vùng</t>
   </si>
@@ -211,68 +211,51 @@
     <t>Cà Mau</t>
   </si>
   <si>
-    <t>Nam Ðịnh</t>
+    <t>Nam Định</t>
   </si>
   <si>
-    <t>Ðiện Biên</t>
+    <t>Điện Biên</t>
   </si>
   <si>
-    <t>Hoà Bình</t>
+    <t>Hòa Bình</t>
   </si>
   <si>
-    <t>Bắc Trung Bộ và Duyên hải miền Trung</t>
+    <t>Thanh Hóa</t>
   </si>
   <si>
-    <t>Thanh Hoá</t>
+    <t>Đà Nẵng</t>
   </si>
   <si>
-    <t>Ðà Nẵng</t>
+    <t>Bình Định</t>
   </si>
   <si>
-    <t>Bình Ðịnh</t>
+    <t>Khánh Hòa</t>
   </si>
   <si>
-    <t>Khánh Hoà</t>
+    <t>Đắk Lắk</t>
   </si>
   <si>
-    <t>Ðắk Lắk</t>
+    <t>Đắk Nông</t>
   </si>
   <si>
-    <t>Ðắk Nông</t>
+    <t>Lâm Đồng</t>
   </si>
   <si>
-    <t>Lâm Ðồng</t>
+    <t>Đồng Nai</t>
   </si>
   <si>
-    <t>Ðông Nam Bộ</t>
+    <t>TP. Hồ Chí Minh</t>
   </si>
   <si>
-    <t>Ðồng Nai</t>
-  </si>
-  <si>
-    <t>TP.Hồ Chí Minh</t>
-  </si>
-  <si>
-    <t>Ðồng bằng sông Cửu Long</t>
-  </si>
-  <si>
-    <t>Ðồng Tháp</t>
+    <t>Đồng Tháp</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -320,12 +303,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -346,9 +326,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2007 - 2010">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -386,7 +366,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2007 - 2010">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -420,7 +400,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -455,10 +434,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2007 - 2010">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -635,21 +613,13 @@
   <dimension ref="A1:F981"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="32.44140625" customWidth="1"/>
-    <col min="2" max="2" width="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="32.21875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -8510,7 +8480,7 @@
     </row>
     <row r="394" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A394" t="s">
-        <v>66</v>
+        <v>31</v>
       </c>
       <c r="B394">
         <v>2011</v>
@@ -8530,7 +8500,7 @@
     </row>
     <row r="395" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A395" t="s">
-        <v>66</v>
+        <v>31</v>
       </c>
       <c r="B395">
         <v>2012</v>
@@ -8550,7 +8520,7 @@
     </row>
     <row r="396" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A396" t="s">
-        <v>66</v>
+        <v>31</v>
       </c>
       <c r="B396">
         <v>2013</v>
@@ -8570,7 +8540,7 @@
     </row>
     <row r="397" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A397" t="s">
-        <v>66</v>
+        <v>31</v>
       </c>
       <c r="B397">
         <v>2014</v>
@@ -8590,7 +8560,7 @@
     </row>
     <row r="398" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A398" t="s">
-        <v>66</v>
+        <v>31</v>
       </c>
       <c r="B398">
         <v>2015</v>
@@ -8610,7 +8580,7 @@
     </row>
     <row r="399" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A399" t="s">
-        <v>66</v>
+        <v>31</v>
       </c>
       <c r="B399">
         <v>2016</v>
@@ -8630,7 +8600,7 @@
     </row>
     <row r="400" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A400" t="s">
-        <v>66</v>
+        <v>31</v>
       </c>
       <c r="B400">
         <v>2017</v>
@@ -8650,7 +8620,7 @@
     </row>
     <row r="401" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A401" t="s">
-        <v>66</v>
+        <v>31</v>
       </c>
       <c r="B401">
         <v>2018</v>
@@ -8670,7 +8640,7 @@
     </row>
     <row r="402" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A402" t="s">
-        <v>66</v>
+        <v>31</v>
       </c>
       <c r="B402">
         <v>2019</v>
@@ -8690,7 +8660,7 @@
     </row>
     <row r="403" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A403" t="s">
-        <v>66</v>
+        <v>31</v>
       </c>
       <c r="B403">
         <v>2020</v>
@@ -8710,7 +8680,7 @@
     </row>
     <row r="404" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A404" t="s">
-        <v>66</v>
+        <v>31</v>
       </c>
       <c r="B404">
         <v>2021</v>
@@ -8730,7 +8700,7 @@
     </row>
     <row r="405" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A405" t="s">
-        <v>66</v>
+        <v>31</v>
       </c>
       <c r="B405">
         <v>2022</v>
@@ -8750,7 +8720,7 @@
     </row>
     <row r="406" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A406" t="s">
-        <v>66</v>
+        <v>31</v>
       </c>
       <c r="B406">
         <v>2023</v>
@@ -8770,7 +8740,7 @@
     </row>
     <row r="407" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A407" t="s">
-        <v>66</v>
+        <v>31</v>
       </c>
       <c r="B407">
         <v>2024</v>
@@ -8790,7 +8760,7 @@
     </row>
     <row r="408" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A408" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B408">
         <v>2011</v>
@@ -8810,7 +8780,7 @@
     </row>
     <row r="409" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A409" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B409">
         <v>2012</v>
@@ -8830,7 +8800,7 @@
     </row>
     <row r="410" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A410" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B410">
         <v>2013</v>
@@ -8850,7 +8820,7 @@
     </row>
     <row r="411" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A411" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B411">
         <v>2014</v>
@@ -8870,7 +8840,7 @@
     </row>
     <row r="412" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A412" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B412">
         <v>2015</v>
@@ -8890,7 +8860,7 @@
     </row>
     <row r="413" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A413" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B413">
         <v>2016</v>
@@ -8910,7 +8880,7 @@
     </row>
     <row r="414" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A414" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B414">
         <v>2017</v>
@@ -8930,7 +8900,7 @@
     </row>
     <row r="415" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A415" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B415">
         <v>2018</v>
@@ -8950,7 +8920,7 @@
     </row>
     <row r="416" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A416" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B416">
         <v>2019</v>
@@ -8970,7 +8940,7 @@
     </row>
     <row r="417" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A417" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B417">
         <v>2020</v>
@@ -8990,7 +8960,7 @@
     </row>
     <row r="418" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A418" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B418">
         <v>2021</v>
@@ -9010,7 +8980,7 @@
     </row>
     <row r="419" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A419" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B419">
         <v>2022</v>
@@ -9030,7 +9000,7 @@
     </row>
     <row r="420" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A420" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B420">
         <v>2023</v>
@@ -9050,7 +9020,7 @@
     </row>
     <row r="421" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A421" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B421">
         <v>2024</v>
@@ -10470,7 +10440,7 @@
     </row>
     <row r="492" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A492" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B492">
         <v>2011</v>
@@ -10490,7 +10460,7 @@
     </row>
     <row r="493" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A493" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B493">
         <v>2012</v>
@@ -10510,7 +10480,7 @@
     </row>
     <row r="494" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A494" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B494">
         <v>2013</v>
@@ -10530,7 +10500,7 @@
     </row>
     <row r="495" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A495" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B495">
         <v>2014</v>
@@ -10550,7 +10520,7 @@
     </row>
     <row r="496" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A496" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B496">
         <v>2015</v>
@@ -10570,7 +10540,7 @@
     </row>
     <row r="497" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A497" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B497">
         <v>2016</v>
@@ -10590,7 +10560,7 @@
     </row>
     <row r="498" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A498" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B498">
         <v>2017</v>
@@ -10610,7 +10580,7 @@
     </row>
     <row r="499" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A499" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B499">
         <v>2018</v>
@@ -10630,7 +10600,7 @@
     </row>
     <row r="500" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A500" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B500">
         <v>2019</v>
@@ -10650,7 +10620,7 @@
     </row>
     <row r="501" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A501" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B501">
         <v>2020</v>
@@ -10670,7 +10640,7 @@
     </row>
     <row r="502" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A502" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B502">
         <v>2021</v>
@@ -10690,7 +10660,7 @@
     </row>
     <row r="503" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A503" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B503">
         <v>2022</v>
@@ -10710,7 +10680,7 @@
     </row>
     <row r="504" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A504" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B504">
         <v>2023</v>
@@ -10730,7 +10700,7 @@
     </row>
     <row r="505" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A505" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B505">
         <v>2024</v>
@@ -11310,7 +11280,7 @@
     </row>
     <row r="534" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A534" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B534">
         <v>2011</v>
@@ -11330,7 +11300,7 @@
     </row>
     <row r="535" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A535" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B535">
         <v>2012</v>
@@ -11350,7 +11320,7 @@
     </row>
     <row r="536" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A536" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B536">
         <v>2013</v>
@@ -11370,7 +11340,7 @@
     </row>
     <row r="537" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A537" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B537">
         <v>2014</v>
@@ -11390,7 +11360,7 @@
     </row>
     <row r="538" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A538" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B538">
         <v>2015</v>
@@ -11410,7 +11380,7 @@
     </row>
     <row r="539" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A539" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B539">
         <v>2016</v>
@@ -11430,7 +11400,7 @@
     </row>
     <row r="540" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A540" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B540">
         <v>2017</v>
@@ -11450,7 +11420,7 @@
     </row>
     <row r="541" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A541" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B541">
         <v>2018</v>
@@ -11470,7 +11440,7 @@
     </row>
     <row r="542" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A542" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B542">
         <v>2019</v>
@@ -11490,7 +11460,7 @@
     </row>
     <row r="543" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A543" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B543">
         <v>2020</v>
@@ -11510,7 +11480,7 @@
     </row>
     <row r="544" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A544" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B544">
         <v>2021</v>
@@ -11530,7 +11500,7 @@
     </row>
     <row r="545" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A545" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B545">
         <v>2022</v>
@@ -11550,7 +11520,7 @@
     </row>
     <row r="546" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A546" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B546">
         <v>2023</v>
@@ -11570,7 +11540,7 @@
     </row>
     <row r="547" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A547" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B547">
         <v>2024</v>
@@ -11870,7 +11840,7 @@
     </row>
     <row r="562" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A562" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B562">
         <v>2011</v>
@@ -11890,7 +11860,7 @@
     </row>
     <row r="563" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A563" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B563">
         <v>2012</v>
@@ -11910,7 +11880,7 @@
     </row>
     <row r="564" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A564" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B564">
         <v>2013</v>
@@ -11930,7 +11900,7 @@
     </row>
     <row r="565" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A565" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B565">
         <v>2014</v>
@@ -11950,7 +11920,7 @@
     </row>
     <row r="566" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A566" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B566">
         <v>2015</v>
@@ -11970,7 +11940,7 @@
     </row>
     <row r="567" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A567" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B567">
         <v>2016</v>
@@ -11990,7 +11960,7 @@
     </row>
     <row r="568" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A568" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B568">
         <v>2017</v>
@@ -12010,7 +11980,7 @@
     </row>
     <row r="569" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A569" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B569">
         <v>2018</v>
@@ -12030,7 +12000,7 @@
     </row>
     <row r="570" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A570" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B570">
         <v>2019</v>
@@ -12050,7 +12020,7 @@
     </row>
     <row r="571" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A571" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B571">
         <v>2020</v>
@@ -12070,7 +12040,7 @@
     </row>
     <row r="572" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A572" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B572">
         <v>2021</v>
@@ -12090,7 +12060,7 @@
     </row>
     <row r="573" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A573" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B573">
         <v>2022</v>
@@ -12110,7 +12080,7 @@
     </row>
     <row r="574" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A574" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B574">
         <v>2023</v>
@@ -12130,7 +12100,7 @@
     </row>
     <row r="575" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A575" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B575">
         <v>2024</v>
@@ -13550,7 +13520,7 @@
     </row>
     <row r="646" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A646" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B646">
         <v>2011</v>
@@ -13570,7 +13540,7 @@
     </row>
     <row r="647" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A647" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B647">
         <v>2012</v>
@@ -13590,7 +13560,7 @@
     </row>
     <row r="648" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A648" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B648">
         <v>2013</v>
@@ -13610,7 +13580,7 @@
     </row>
     <row r="649" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A649" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B649">
         <v>2014</v>
@@ -13630,7 +13600,7 @@
     </row>
     <row r="650" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A650" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B650">
         <v>2015</v>
@@ -13650,7 +13620,7 @@
     </row>
     <row r="651" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A651" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B651">
         <v>2016</v>
@@ -13670,7 +13640,7 @@
     </row>
     <row r="652" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A652" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B652">
         <v>2017</v>
@@ -13690,7 +13660,7 @@
     </row>
     <row r="653" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A653" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B653">
         <v>2018</v>
@@ -13710,7 +13680,7 @@
     </row>
     <row r="654" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A654" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B654">
         <v>2019</v>
@@ -13730,7 +13700,7 @@
     </row>
     <row r="655" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A655" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B655">
         <v>2020</v>
@@ -13750,7 +13720,7 @@
     </row>
     <row r="656" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A656" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B656">
         <v>2021</v>
@@ -13770,7 +13740,7 @@
     </row>
     <row r="657" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A657" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B657">
         <v>2022</v>
@@ -13790,7 +13760,7 @@
     </row>
     <row r="658" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A658" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B658">
         <v>2023</v>
@@ -13810,7 +13780,7 @@
     </row>
     <row r="659" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A659" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B659">
         <v>2024</v>
@@ -13830,7 +13800,7 @@
     </row>
     <row r="660" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A660" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B660">
         <v>2011</v>
@@ -13850,7 +13820,7 @@
     </row>
     <row r="661" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A661" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B661">
         <v>2012</v>
@@ -13870,7 +13840,7 @@
     </row>
     <row r="662" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A662" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B662">
         <v>2013</v>
@@ -13890,7 +13860,7 @@
     </row>
     <row r="663" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A663" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B663">
         <v>2014</v>
@@ -13910,7 +13880,7 @@
     </row>
     <row r="664" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A664" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B664">
         <v>2015</v>
@@ -13930,7 +13900,7 @@
     </row>
     <row r="665" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A665" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B665">
         <v>2016</v>
@@ -13950,7 +13920,7 @@
     </row>
     <row r="666" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A666" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B666">
         <v>2017</v>
@@ -13970,7 +13940,7 @@
     </row>
     <row r="667" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A667" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B667">
         <v>2018</v>
@@ -13990,7 +13960,7 @@
     </row>
     <row r="668" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A668" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B668">
         <v>2019</v>
@@ -14010,7 +13980,7 @@
     </row>
     <row r="669" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A669" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B669">
         <v>2020</v>
@@ -14030,7 +14000,7 @@
     </row>
     <row r="670" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A670" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B670">
         <v>2021</v>
@@ -14050,7 +14020,7 @@
     </row>
     <row r="671" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A671" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B671">
         <v>2022</v>
@@ -14070,7 +14040,7 @@
     </row>
     <row r="672" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A672" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B672">
         <v>2023</v>
@@ -14090,7 +14060,7 @@
     </row>
     <row r="673" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A673" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B673">
         <v>2024</v>
@@ -14110,7 +14080,7 @@
     </row>
     <row r="674" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A674" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B674">
         <v>2011</v>
@@ -14130,7 +14100,7 @@
     </row>
     <row r="675" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A675" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B675">
         <v>2012</v>
@@ -14150,7 +14120,7 @@
     </row>
     <row r="676" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A676" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B676">
         <v>2013</v>
@@ -14170,7 +14140,7 @@
     </row>
     <row r="677" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A677" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B677">
         <v>2014</v>
@@ -14190,7 +14160,7 @@
     </row>
     <row r="678" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A678" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B678">
         <v>2015</v>
@@ -14210,7 +14180,7 @@
     </row>
     <row r="679" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A679" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B679">
         <v>2016</v>
@@ -14230,7 +14200,7 @@
     </row>
     <row r="680" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A680" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B680">
         <v>2017</v>
@@ -14250,7 +14220,7 @@
     </row>
     <row r="681" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A681" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B681">
         <v>2018</v>
@@ -14270,7 +14240,7 @@
     </row>
     <row r="682" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A682" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B682">
         <v>2019</v>
@@ -14290,7 +14260,7 @@
     </row>
     <row r="683" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A683" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B683">
         <v>2020</v>
@@ -14310,7 +14280,7 @@
     </row>
     <row r="684" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A684" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B684">
         <v>2021</v>
@@ -14330,7 +14300,7 @@
     </row>
     <row r="685" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A685" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B685">
         <v>2022</v>
@@ -14350,7 +14320,7 @@
     </row>
     <row r="686" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A686" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B686">
         <v>2023</v>
@@ -14370,7 +14340,7 @@
     </row>
     <row r="687" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A687" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B687">
         <v>2024</v>
@@ -14390,7 +14360,7 @@
     </row>
     <row r="688" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A688" t="s">
-        <v>74</v>
+        <v>45</v>
       </c>
       <c r="B688">
         <v>2011</v>
@@ -14410,7 +14380,7 @@
     </row>
     <row r="689" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A689" t="s">
-        <v>74</v>
+        <v>45</v>
       </c>
       <c r="B689">
         <v>2012</v>
@@ -14430,7 +14400,7 @@
     </row>
     <row r="690" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A690" t="s">
-        <v>74</v>
+        <v>45</v>
       </c>
       <c r="B690">
         <v>2013</v>
@@ -14450,7 +14420,7 @@
     </row>
     <row r="691" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A691" t="s">
-        <v>74</v>
+        <v>45</v>
       </c>
       <c r="B691">
         <v>2014</v>
@@ -14470,7 +14440,7 @@
     </row>
     <row r="692" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A692" t="s">
-        <v>74</v>
+        <v>45</v>
       </c>
       <c r="B692">
         <v>2015</v>
@@ -14490,7 +14460,7 @@
     </row>
     <row r="693" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A693" t="s">
-        <v>74</v>
+        <v>45</v>
       </c>
       <c r="B693">
         <v>2016</v>
@@ -14510,7 +14480,7 @@
     </row>
     <row r="694" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A694" t="s">
-        <v>74</v>
+        <v>45</v>
       </c>
       <c r="B694">
         <v>2017</v>
@@ -14530,7 +14500,7 @@
     </row>
     <row r="695" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A695" t="s">
-        <v>74</v>
+        <v>45</v>
       </c>
       <c r="B695">
         <v>2018</v>
@@ -14550,7 +14520,7 @@
     </row>
     <row r="696" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A696" t="s">
-        <v>74</v>
+        <v>45</v>
       </c>
       <c r="B696">
         <v>2019</v>
@@ -14570,7 +14540,7 @@
     </row>
     <row r="697" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A697" t="s">
-        <v>74</v>
+        <v>45</v>
       </c>
       <c r="B697">
         <v>2020</v>
@@ -14590,7 +14560,7 @@
     </row>
     <row r="698" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A698" t="s">
-        <v>74</v>
+        <v>45</v>
       </c>
       <c r="B698">
         <v>2021</v>
@@ -14610,7 +14580,7 @@
     </row>
     <row r="699" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A699" t="s">
-        <v>74</v>
+        <v>45</v>
       </c>
       <c r="B699">
         <v>2022</v>
@@ -14630,7 +14600,7 @@
     </row>
     <row r="700" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A700" t="s">
-        <v>74</v>
+        <v>45</v>
       </c>
       <c r="B700">
         <v>2023</v>
@@ -14650,7 +14620,7 @@
     </row>
     <row r="701" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A701" t="s">
-        <v>74</v>
+        <v>45</v>
       </c>
       <c r="B701">
         <v>2024</v>
@@ -15510,7 +15480,7 @@
     </row>
     <row r="744" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A744" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B744">
         <v>2011</v>
@@ -15530,7 +15500,7 @@
     </row>
     <row r="745" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A745" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B745">
         <v>2012</v>
@@ -15550,7 +15520,7 @@
     </row>
     <row r="746" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A746" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B746">
         <v>2013</v>
@@ -15570,7 +15540,7 @@
     </row>
     <row r="747" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A747" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B747">
         <v>2014</v>
@@ -15590,7 +15560,7 @@
     </row>
     <row r="748" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A748" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B748">
         <v>2015</v>
@@ -15610,7 +15580,7 @@
     </row>
     <row r="749" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A749" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B749">
         <v>2016</v>
@@ -15630,7 +15600,7 @@
     </row>
     <row r="750" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A750" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B750">
         <v>2017</v>
@@ -15650,7 +15620,7 @@
     </row>
     <row r="751" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A751" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B751">
         <v>2018</v>
@@ -15670,7 +15640,7 @@
     </row>
     <row r="752" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A752" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B752">
         <v>2019</v>
@@ -15690,7 +15660,7 @@
     </row>
     <row r="753" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A753" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B753">
         <v>2020</v>
@@ -15710,7 +15680,7 @@
     </row>
     <row r="754" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A754" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B754">
         <v>2021</v>
@@ -15730,7 +15700,7 @@
     </row>
     <row r="755" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A755" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B755">
         <v>2022</v>
@@ -15750,7 +15720,7 @@
     </row>
     <row r="756" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A756" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B756">
         <v>2023</v>
@@ -15770,7 +15740,7 @@
     </row>
     <row r="757" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A757" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B757">
         <v>2024</v>
@@ -16070,7 +16040,7 @@
     </row>
     <row r="772" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A772" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B772">
         <v>2011</v>
@@ -16090,7 +16060,7 @@
     </row>
     <row r="773" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A773" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B773">
         <v>2012</v>
@@ -16110,7 +16080,7 @@
     </row>
     <row r="774" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A774" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B774">
         <v>2013</v>
@@ -16130,7 +16100,7 @@
     </row>
     <row r="775" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A775" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B775">
         <v>2014</v>
@@ -16150,7 +16120,7 @@
     </row>
     <row r="776" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A776" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B776">
         <v>2015</v>
@@ -16170,7 +16140,7 @@
     </row>
     <row r="777" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A777" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B777">
         <v>2016</v>
@@ -16190,7 +16160,7 @@
     </row>
     <row r="778" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A778" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B778">
         <v>2017</v>
@@ -16210,7 +16180,7 @@
     </row>
     <row r="779" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A779" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B779">
         <v>2018</v>
@@ -16230,7 +16200,7 @@
     </row>
     <row r="780" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A780" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B780">
         <v>2019</v>
@@ -16250,7 +16220,7 @@
     </row>
     <row r="781" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A781" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B781">
         <v>2020</v>
@@ -16270,7 +16240,7 @@
     </row>
     <row r="782" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A782" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B782">
         <v>2021</v>
@@ -16290,7 +16260,7 @@
     </row>
     <row r="783" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A783" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B783">
         <v>2022</v>
@@ -16310,7 +16280,7 @@
     </row>
     <row r="784" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A784" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B784">
         <v>2023</v>
@@ -16330,7 +16300,7 @@
     </row>
     <row r="785" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A785" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B785">
         <v>2024</v>
@@ -16350,7 +16320,7 @@
     </row>
     <row r="786" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A786" t="s">
-        <v>77</v>
+        <v>50</v>
       </c>
       <c r="B786">
         <v>2011</v>
@@ -16370,7 +16340,7 @@
     </row>
     <row r="787" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A787" t="s">
-        <v>77</v>
+        <v>50</v>
       </c>
       <c r="B787">
         <v>2012</v>
@@ -16390,7 +16360,7 @@
     </row>
     <row r="788" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A788" t="s">
-        <v>77</v>
+        <v>50</v>
       </c>
       <c r="B788">
         <v>2013</v>
@@ -16410,7 +16380,7 @@
     </row>
     <row r="789" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A789" t="s">
-        <v>77</v>
+        <v>50</v>
       </c>
       <c r="B789">
         <v>2014</v>
@@ -16430,7 +16400,7 @@
     </row>
     <row r="790" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A790" t="s">
-        <v>77</v>
+        <v>50</v>
       </c>
       <c r="B790">
         <v>2015</v>
@@ -16450,7 +16420,7 @@
     </row>
     <row r="791" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A791" t="s">
-        <v>77</v>
+        <v>50</v>
       </c>
       <c r="B791">
         <v>2016</v>
@@ -16470,7 +16440,7 @@
     </row>
     <row r="792" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A792" t="s">
-        <v>77</v>
+        <v>50</v>
       </c>
       <c r="B792">
         <v>2017</v>
@@ -16490,7 +16460,7 @@
     </row>
     <row r="793" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A793" t="s">
-        <v>77</v>
+        <v>50</v>
       </c>
       <c r="B793">
         <v>2018</v>
@@ -16510,7 +16480,7 @@
     </row>
     <row r="794" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A794" t="s">
-        <v>77</v>
+        <v>50</v>
       </c>
       <c r="B794">
         <v>2019</v>
@@ -16530,7 +16500,7 @@
     </row>
     <row r="795" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A795" t="s">
-        <v>77</v>
+        <v>50</v>
       </c>
       <c r="B795">
         <v>2020</v>
@@ -16550,7 +16520,7 @@
     </row>
     <row r="796" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A796" t="s">
-        <v>77</v>
+        <v>50</v>
       </c>
       <c r="B796">
         <v>2021</v>
@@ -16570,7 +16540,7 @@
     </row>
     <row r="797" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A797" t="s">
-        <v>77</v>
+        <v>50</v>
       </c>
       <c r="B797">
         <v>2022</v>
@@ -16590,7 +16560,7 @@
     </row>
     <row r="798" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A798" t="s">
-        <v>77</v>
+        <v>50</v>
       </c>
       <c r="B798">
         <v>2023</v>
@@ -16610,7 +16580,7 @@
     </row>
     <row r="799" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A799" t="s">
-        <v>77</v>
+        <v>50</v>
       </c>
       <c r="B799">
         <v>2024</v>
@@ -18030,7 +18000,7 @@
     </row>
     <row r="870" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A870" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B870">
         <v>2011</v>
@@ -18050,7 +18020,7 @@
     </row>
     <row r="871" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A871" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B871">
         <v>2012</v>
@@ -18070,7 +18040,7 @@
     </row>
     <row r="872" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A872" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B872">
         <v>2013</v>
@@ -18090,7 +18060,7 @@
     </row>
     <row r="873" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A873" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B873">
         <v>2014</v>
@@ -18110,7 +18080,7 @@
     </row>
     <row r="874" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A874" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B874">
         <v>2015</v>
@@ -18130,7 +18100,7 @@
     </row>
     <row r="875" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A875" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B875">
         <v>2016</v>
@@ -18150,7 +18120,7 @@
     </row>
     <row r="876" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A876" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B876">
         <v>2017</v>
@@ -18170,7 +18140,7 @@
     </row>
     <row r="877" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A877" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B877">
         <v>2018</v>
@@ -18190,7 +18160,7 @@
     </row>
     <row r="878" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A878" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B878">
         <v>2019</v>
@@ -18210,7 +18180,7 @@
     </row>
     <row r="879" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A879" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B879">
         <v>2020</v>
@@ -18230,7 +18200,7 @@
     </row>
     <row r="880" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A880" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B880">
         <v>2021</v>
@@ -18250,7 +18220,7 @@
     </row>
     <row r="881" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A881" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B881">
         <v>2022</v>
@@ -18270,7 +18240,7 @@
     </row>
     <row r="882" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A882" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B882">
         <v>2023</v>
@@ -18290,7 +18260,7 @@
     </row>
     <row r="883" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A883" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B883">
         <v>2024</v>
@@ -20269,6 +20239,6 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>